<commit_message>
assign student to exam fixed to specific school
</commit_message>
<xml_diff>
--- a/public/files/exports/nilai-siswa.xlsx
+++ b/public/files/exports/nilai-siswa.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Nilai Siswa" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="ujian 1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="ujian 2" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>NIS</t>
   </si>
@@ -31,12 +32,6 @@
     <t>KKM</t>
   </si>
   <si>
-    <t>Nilai 1</t>
-  </si>
-  <si>
-    <t>Nilai 2</t>
-  </si>
-  <si>
     <t>0001010</t>
   </si>
   <si>
@@ -50,9 +45,6 @@
   </si>
   <si>
     <t>ujian 1</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -433,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,37 +447,76 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>70</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>